<commit_message>
Add level of scope
</commit_message>
<xml_diff>
--- a/dataset/label/legality.xlsx
+++ b/dataset/label/legality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachary/projects/DeepWTO/dataset/label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2298260-8E14-444E-AD0F-54AA954748CF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4EA6A-4B45-EC42-A14C-B5A80F878354}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="2" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
   </bookViews>
   <sheets>
     <sheet name="factual" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
   <si>
     <t>The dual retail system for beef (including the obligation for department stores and supermarkets authorized to sell imported beef to hold a separate display, and the obligation for foreign beef shops to bear a sign "Specialized Imported Beef Stores")</t>
   </si>
@@ -285,6 +285,18 @@
   </si>
   <si>
     <t>United States — Import Measures on Certain Products from the European Communities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> as such led to violations of Articles II:1(a) and II:1(b)</t>
+  </si>
+  <si>
+    <t>3 March Measure</t>
+  </si>
+  <si>
+    <t>II:1(b)</t>
+  </si>
+  <si>
+    <t>II:1(a)</t>
   </si>
 </sst>
 </file>
@@ -723,7 +735,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,8 +788,12 @@
       <c r="A5" s="10">
         <v>165</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="10">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
@@ -799,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119486A2-4A2B-D247-A44C-CAB1B05D3F70}">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView zoomScale="136" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1381,6 +1397,20 @@
       <c r="B28" t="s">
         <v>85</v>
       </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1675,7 +1705,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877F0A9-3B5A-A944-83AA-53E65EA9EAD4}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add 166 and 170
</commit_message>
<xml_diff>
--- a/dataset/label/legality.xlsx
+++ b/dataset/label/legality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachary/projects/DeepWTO/dataset/label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC4EA6A-4B45-EC42-A14C-B5A80F878354}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFB5D19-B488-894C-B518-D00D889785E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="103">
   <si>
     <t>The dual retail system for beef (including the obligation for department stores and supermarkets authorized to sell imported beef to hold a separate display, and the obligation for foreign beef shops to bear a sign "Specialized Imported Beef Stores")</t>
   </si>
@@ -287,9 +287,6 @@
     <t>United States — Import Measures on Certain Products from the European Communities</t>
   </si>
   <si>
-    <t xml:space="preserve"> as such led to violations of Articles II:1(a) and II:1(b)</t>
-  </si>
-  <si>
     <t>3 March Measure</t>
   </si>
   <si>
@@ -297,6 +294,48 @@
   </si>
   <si>
     <t>II:1(a)</t>
+  </si>
+  <si>
+    <t>GATT I</t>
+  </si>
+  <si>
+    <t>DSU 3.7</t>
+  </si>
+  <si>
+    <t>DSU 22.6</t>
+  </si>
+  <si>
+    <t>DSU 23.2(c)</t>
+  </si>
+  <si>
+    <t>DSU 23.1</t>
+  </si>
+  <si>
+    <t>one Panelist is of the view that such increased bonding requirements of the 3 March Measure rather violated Article XI of GATT</t>
+  </si>
+  <si>
+    <t>DSU 21.5</t>
+  </si>
+  <si>
+    <t>3 March Measure; the United States made a unilateral determination that the EC implementing measure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSU  23.2(a) </t>
+  </si>
+  <si>
+    <t>The increased bonding requirements of the 3 March Measure</t>
+  </si>
+  <si>
+    <t>the 3 March Measure constituted a suspension of concessions or other obligations</t>
+  </si>
+  <si>
+    <t>Canada – Term of Patent Protection</t>
+  </si>
+  <si>
+    <t>Section 45 of Canada's Patent Act</t>
+  </si>
+  <si>
+    <t>TRIPS 33</t>
   </si>
 </sst>
 </file>
@@ -333,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +421,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -395,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -411,6 +456,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -418,6 +466,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4690C8-E376-F64C-83C0-2939844C6F10}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,14 +845,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>166</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="13">
         <v>7</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="13">
         <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="15">
+        <v>170</v>
+      </c>
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+      <c r="C7" s="15">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -813,10 +873,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119486A2-4A2B-D247-A44C-CAB1B05D3F70}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,7 +885,7 @@
     <col min="3" max="3" width="230.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="86.5" customWidth="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="53.1640625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="24.83203125" customWidth="1"/>
   </cols>
@@ -846,7 +906,9 @@
       <c r="E1" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="G1" s="8" t="s">
         <v>7</v>
       </c>
@@ -1394,306 +1456,503 @@
       <c r="A28" s="10">
         <v>165</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>165</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E29" s="10">
+        <v>1</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>165</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>165</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="10">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
+        <v>165</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D32" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E32" s="10">
+        <v>1</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>165</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E33" s="10">
+        <v>1</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>165</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="10">
+        <v>1</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>165</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>165</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="10">
+        <v>1</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
+        <v>165</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="13">
+        <v>166</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="13">
+        <v>166</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="13">
+        <v>0</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="13">
+        <v>166</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="13">
+        <v>0</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="13">
+        <v>166</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" s="13">
+        <v>0</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="13">
+        <v>166</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="13">
+        <v>0</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="13">
+        <v>166</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E43" s="13">
+        <v>0</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+    </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="12">
+      <c r="A44" s="13">
         <v>166</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="12" t="s">
+      <c r="C44" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E44" s="13">
+        <v>1</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="13">
+        <v>166</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="12">
-        <v>0</v>
-      </c>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="12">
+      <c r="E45" s="13">
+        <v>1</v>
+      </c>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="13">
         <v>166</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B46" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="12">
-        <v>0</v>
-      </c>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="12">
+      <c r="C46" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="13">
+        <v>1</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="13">
         <v>166</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B47" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="12">
-        <v>0</v>
-      </c>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="12">
+      <c r="C47" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E47" s="13">
+        <v>1</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="13">
         <v>166</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B48" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="12">
-        <v>0</v>
-      </c>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="12">
+      <c r="C48" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E48" s="13">
+        <v>1</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="13">
         <v>166</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" s="12">
-        <v>0</v>
-      </c>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="12">
+      <c r="C49" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="13">
+        <v>1</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="13">
         <v>166</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E49" s="12">
-        <v>0</v>
-      </c>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="12">
+      <c r="C50" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="13">
+        <v>1</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="13">
         <v>166</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B51" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="12">
-        <v>1</v>
-      </c>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-    </row>
-    <row r="51" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A51" s="12">
-        <v>166</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>84</v>
-      </c>
       <c r="C51" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E51" s="12">
-        <v>1</v>
-      </c>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-    </row>
-    <row r="52" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A52" s="12">
-        <v>166</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" s="12">
-        <v>1</v>
-      </c>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="12">
-        <v>166</v>
-      </c>
-      <c r="B53" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E53" s="12">
-        <v>1</v>
-      </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="12">
-        <v>166</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" s="12">
-        <v>1</v>
-      </c>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="12">
-        <v>166</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" s="12">
-        <v>1</v>
-      </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="12">
-        <v>166</v>
-      </c>
-      <c r="B56" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C56" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D56" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E56" s="12">
-        <v>1</v>
-      </c>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="12">
-        <v>166</v>
-      </c>
-      <c r="B57" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C57" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="12" t="s">
+      <c r="D51" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="12">
-        <v>1</v>
-      </c>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
+      <c r="E51" s="13">
+        <v>1</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="15">
+        <v>170</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="15">
+        <v>1</v>
+      </c>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1703,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877F0A9-3B5A-A944-83AA-53E65EA9EAD4}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="143" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1750,7 +2009,7 @@
       <c r="A2" s="2">
         <v>161</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1770,7 +2029,7 @@
       <c r="A3" s="2">
         <v>161</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1790,7 +2049,7 @@
       <c r="A4" s="2">
         <v>161</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1810,7 +2069,7 @@
       <c r="A5" s="2">
         <v>161</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1950,215 +2209,425 @@
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>165</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C12" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>165</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>165</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>165</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>165</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>165</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>165</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>165</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>165</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="10">
+        <v>1</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>165</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>166</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="13">
         <v>0</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="12">
+      <c r="A23" s="13">
         <v>166</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="13">
         <v>0</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="12">
+      <c r="A24" s="13">
         <v>166</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-    </row>
-    <row r="25" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="12">
+      <c r="E24" s="13">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13">
         <v>166</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="12">
-        <v>1</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-    </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="12">
+      <c r="E25" s="13">
+        <v>1</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13">
         <v>166</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="12">
-        <v>1</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="E26" s="13">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="12">
+      <c r="A27" s="13">
         <v>166</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="12">
-        <v>1</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="E27" s="13">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="12">
+      <c r="A28" s="13">
         <v>166</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="12">
-        <v>1</v>
-      </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="E28" s="13">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="12">
+      <c r="A29" s="13">
         <v>166</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="13">
         <v>0</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="12">
+      <c r="A30" s="13">
         <v>166</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="12">
-        <v>1</v>
-      </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="E30" s="13">
+        <v>1</v>
+      </c>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="12">
+      <c r="A31" s="13">
         <v>166</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="E31" s="13">
+        <v>1</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="15">
+        <v>170</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" s="15">
+        <v>1</v>
+      </c>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 174 and 175
</commit_message>
<xml_diff>
--- a/dataset/label/legality.xlsx
+++ b/dataset/label/legality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachary/projects/DeepWTO/dataset/label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFB5D19-B488-894C-B518-D00D889785E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD57EA1-DC35-134D-A61A-369A90391096}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
   <si>
     <t>The dual retail system for beef (including the obligation for department stores and supermarkets authorized to sell imported beef to hold a separate display, and the obligation for foreign beef shops to bear a sign "Specialized Imported Beef Stores")</t>
   </si>
@@ -336,6 +336,45 @@
   </si>
   <si>
     <t>TRIPS 33</t>
+  </si>
+  <si>
+    <t>European Communities — Protection of Trademarks and Geographical Indications for Agricultural Products and Foodstuffs</t>
+  </si>
+  <si>
+    <t>the Regulation</t>
+  </si>
+  <si>
+    <t>TRIPS 3.1</t>
+  </si>
+  <si>
+    <t>TRIPS 2.1</t>
+  </si>
+  <si>
+    <t>TRIPS 16.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIPS 24.3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIPS 24.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRIPS 4 </t>
+  </si>
+  <si>
+    <t>TRIPS 22.2</t>
+  </si>
+  <si>
+    <t>TRIPS 1.1</t>
+  </si>
+  <si>
+    <t>India — Measures Affecting Trade and Investment in the Motor Vehicle Sector</t>
+  </si>
+  <si>
+    <t>imposing on automotive manufacturers, under the terms of Public Notice No. 60 and the MOUs signed thereunder, an obligation to use a certain proportion of local parts and components in the manufacture of cars and automotive vehicles ("indigenization" condition)</t>
+  </si>
+  <si>
+    <t>imposing, in the context of the trade balancing condition under the terms of Public Notice No. 60 and the MOUs signed thereunder, an obligation to offset the amount of any purchases of previously imported restricted kits and components on the Indian market, by exports of equivalent value;</t>
   </si>
 </sst>
 </file>
@@ -372,7 +411,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +466,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -440,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -450,6 +501,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -467,6 +519,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -781,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4690C8-E376-F64C-83C0-2939844C6F10}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,47 +878,69 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="8">
         <v>163</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>5</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>165</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
         <v>5</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="11">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
+      <c r="A6" s="14">
         <v>166</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="14">
         <v>7</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="14">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="15">
+      <c r="A7" s="16">
         <v>170</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="16">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="16">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>174</v>
+      </c>
+      <c r="B8" s="17">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
+        <v>175</v>
+      </c>
+      <c r="B9" s="18">
+        <v>9</v>
+      </c>
+      <c r="C9" s="18">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -873,16 +950,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119486A2-4A2B-D247-A44C-CAB1B05D3F70}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="89.6640625" customWidth="1"/>
-    <col min="3" max="3" width="230.83203125" customWidth="1"/>
+    <col min="2" max="2" width="98.6640625" customWidth="1"/>
+    <col min="3" max="3" width="249" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="86.5" customWidth="1"/>
     <col min="6" max="6" width="53.1640625" customWidth="1"/>
@@ -891,28 +968,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1433,526 +1510,750 @@
       <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
+      <c r="A27" s="8">
         <v>163</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="8">
         <v>0</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="10">
+      <c r="A28" s="11">
         <v>165</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="10">
-        <v>1</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="E28" s="11">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="10">
+      <c r="A29" s="11">
         <v>165</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="10">
-        <v>1</v>
-      </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
+      <c r="E29" s="11">
+        <v>1</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="10">
+      <c r="A30" s="11">
         <v>165</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="10">
-        <v>1</v>
-      </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
+      <c r="E30" s="11">
+        <v>1</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10">
+      <c r="A31" s="11">
         <v>165</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="10">
-        <v>1</v>
-      </c>
-      <c r="F31" s="11" t="s">
+      <c r="E31" s="11">
+        <v>1</v>
+      </c>
+      <c r="F31" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="10">
+      <c r="A32" s="11">
         <v>165</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="10">
-        <v>1</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
+      <c r="E32" s="11">
+        <v>1</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="10">
+      <c r="A33" s="11">
         <v>165</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E33" s="10">
-        <v>1</v>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="E33" s="11">
+        <v>1</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="10">
+      <c r="A34" s="11">
         <v>165</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="10">
-        <v>1</v>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
+      <c r="E34" s="11">
+        <v>1</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="10">
+      <c r="A35" s="11">
         <v>165</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="10">
-        <v>1</v>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
+      <c r="E35" s="11">
+        <v>1</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="10">
+      <c r="A36" s="11">
         <v>165</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C36" s="10" t="s">
+      <c r="C36" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E36" s="10">
-        <v>1</v>
-      </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
+      <c r="E36" s="11">
+        <v>1</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="10">
+      <c r="A37" s="11">
         <v>165</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C37" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="10">
-        <v>1</v>
-      </c>
-      <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
-      <c r="H37" s="10"/>
+      <c r="E37" s="11">
+        <v>1</v>
+      </c>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
+      <c r="A38" s="14">
         <v>166</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="14">
         <v>0</v>
       </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="13">
+      <c r="A39" s="14">
         <v>166</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="14">
         <v>0</v>
       </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13">
+      <c r="A40" s="14">
         <v>166</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="14">
         <v>0</v>
       </c>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13">
+      <c r="A41" s="14">
         <v>166</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="14">
         <v>0</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13">
+      <c r="A42" s="14">
         <v>166</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="14">
         <v>0</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="13">
+      <c r="A43" s="14">
         <v>166</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="14">
         <v>0</v>
       </c>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="13">
+      <c r="A44" s="14">
         <v>166</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="D44" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E44" s="13">
-        <v>1</v>
-      </c>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
+      <c r="E44" s="14">
+        <v>1</v>
+      </c>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13">
+      <c r="A45" s="14">
         <v>166</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E45" s="13">
-        <v>1</v>
-      </c>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
+      <c r="E45" s="14">
+        <v>1</v>
+      </c>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13">
+      <c r="A46" s="14">
         <v>166</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D46" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E46" s="13">
-        <v>1</v>
-      </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
+      <c r="E46" s="14">
+        <v>1</v>
+      </c>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="13">
+      <c r="A47" s="14">
         <v>166</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="13">
-        <v>1</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
+      <c r="E47" s="14">
+        <v>1</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
     </row>
     <row r="48" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13">
+      <c r="A48" s="14">
         <v>166</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="13">
-        <v>1</v>
-      </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
+      <c r="E48" s="14">
+        <v>1</v>
+      </c>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13">
+      <c r="A49" s="14">
         <v>166</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E49" s="13">
-        <v>1</v>
-      </c>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
+      <c r="E49" s="14">
+        <v>1</v>
+      </c>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="13">
+      <c r="A50" s="14">
         <v>166</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="13">
-        <v>1</v>
-      </c>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
+      <c r="E50" s="14">
+        <v>1</v>
+      </c>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="13">
+      <c r="A51" s="14">
         <v>166</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E51" s="13">
-        <v>1</v>
-      </c>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
+      <c r="E51" s="14">
+        <v>1</v>
+      </c>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="15">
+      <c r="A52" s="16">
         <v>170</v>
       </c>
-      <c r="B52" s="15" t="s">
+      <c r="B52" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E52" s="15">
-        <v>1</v>
-      </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15"/>
+      <c r="E52" s="16">
+        <v>1</v>
+      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="17">
+        <v>174</v>
+      </c>
+      <c r="B53" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="17">
+        <v>1</v>
+      </c>
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="17">
+        <v>174</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="17">
+        <v>0</v>
+      </c>
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="17">
+        <v>174</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="17">
+        <v>1</v>
+      </c>
+      <c r="F55" s="17"/>
+      <c r="G55" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" s="17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="17">
+        <v>174</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E56" s="17">
+        <v>1</v>
+      </c>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="17">
+        <v>174</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="E57" s="17">
+        <v>0</v>
+      </c>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="17">
+        <v>174</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E58" s="17">
+        <v>0</v>
+      </c>
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="17">
+        <v>174</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E59" s="17">
+        <v>0</v>
+      </c>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="17">
+        <v>174</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="17">
+        <v>0</v>
+      </c>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="17">
+        <v>174</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" s="17">
+        <v>0</v>
+      </c>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="18">
+        <v>175</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="18">
+        <v>1</v>
+      </c>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="18">
+        <v>175</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="18">
+        <v>1</v>
+      </c>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1962,10 +2263,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877F0A9-3B5A-A944-83AA-53E65EA9EAD4}">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2009,7 +2310,7 @@
       <c r="A2" s="2">
         <v>161</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2029,7 +2330,7 @@
       <c r="A3" s="2">
         <v>161</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2049,7 +2350,7 @@
       <c r="A4" s="2">
         <v>161</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -2069,7 +2370,7 @@
       <c r="A5" s="2">
         <v>161</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -2210,424 +2511,427 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>165</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="10">
-        <v>1</v>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
+      <c r="E12" s="11">
+        <v>1</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="10">
+      <c r="A13" s="11">
         <v>165</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="11">
         <v>0</v>
       </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
+      <c r="A14" s="11">
         <v>165</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="10">
-        <v>1</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="E14" s="11">
+        <v>1</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10">
+      <c r="A15" s="11">
         <v>165</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="11">
         <v>0</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10">
+      <c r="A16" s="11">
         <v>165</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="11">
         <v>0</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="10">
+      <c r="A17" s="11">
         <v>165</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="10">
-        <v>1</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
+      <c r="E17" s="11">
+        <v>1</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="10">
+      <c r="A18" s="11">
         <v>165</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E18" s="10">
-        <v>1</v>
-      </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
+      <c r="E18" s="11">
+        <v>1</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
+      <c r="A19" s="11">
         <v>165</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="10">
-        <v>1</v>
-      </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
+      <c r="E19" s="11">
+        <v>1</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>165</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="10">
-        <v>1</v>
-      </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
+      <c r="E20" s="11">
+        <v>1</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="10">
+      <c r="A21" s="11">
         <v>165</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="10">
-        <v>1</v>
-      </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
+      <c r="E21" s="11">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="13">
+      <c r="A22" s="14">
         <v>166</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="14">
         <v>0</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="13">
+      <c r="A23" s="14">
         <v>166</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="14">
         <v>0</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>166</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="13">
-        <v>1</v>
-      </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
+      <c r="E24" s="14">
+        <v>1</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13">
+      <c r="A25" s="14">
         <v>166</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="13">
-        <v>1</v>
-      </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
+      <c r="E25" s="14">
+        <v>1</v>
+      </c>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>166</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="13">
-        <v>1</v>
-      </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
+      <c r="E26" s="14">
+        <v>1</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>166</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="13">
-        <v>1</v>
-      </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="E27" s="14">
+        <v>1</v>
+      </c>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>166</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="13">
-        <v>1</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
+      <c r="E28" s="14">
+        <v>1</v>
+      </c>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>166</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="14">
         <v>0</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
+      <c r="A30" s="14">
         <v>166</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="13">
-        <v>1</v>
-      </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="E30" s="14">
+        <v>1</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
+      <c r="A31" s="14">
         <v>166</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="13">
-        <v>1</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="E31" s="14">
+        <v>1</v>
+      </c>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="15">
+      <c r="A32" s="16">
         <v>170</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E32" s="15">
-        <v>1</v>
-      </c>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
+      <c r="E32" s="16">
+        <v>1</v>
+      </c>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add 177 linked with178
</commit_message>
<xml_diff>
--- a/dataset/label/legality.xlsx
+++ b/dataset/label/legality.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachary/projects/DeepWTO/dataset/label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD57EA1-DC35-134D-A61A-369A90391096}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B8071D-B229-9542-99AC-E74494D2C8C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="1" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
   </bookViews>
   <sheets>
     <sheet name="factual" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="123">
   <si>
     <t>The dual retail system for beef (including the obligation for department stores and supermarkets authorized to sell imported beef to hold a separate display, and the obligation for foreign beef shops to bear a sign "Specialized Imported Beef Stores")</t>
   </si>
@@ -375,13 +375,34 @@
   </si>
   <si>
     <t>imposing, in the context of the trade balancing condition under the terms of Public Notice No. 60 and the MOUs signed thereunder, an obligation to offset the amount of any purchases of previously imported restricted kits and components on the Indian market, by exports of equivalent value;</t>
+  </si>
+  <si>
+    <t>United States — Safeguard Measure on Imports of Fresh, Chilled or Frozen Lamb from New Zealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SA 4.1(c) </t>
+  </si>
+  <si>
+    <t>the imposition of a definitive safeguard measure by the United States on imports of fresh, chilled and frozen lamb meat, imported under subheadings 0204.10.00, 0204.22.20, 0204.23.20, 0204.30.00, 0204.42.20 and 0204.43.20 of the Harmonized Tariff Schedule of the United States.</t>
+  </si>
+  <si>
+    <t>SA 4.1(b)</t>
+  </si>
+  <si>
+    <t>supplementary</t>
+  </si>
+  <si>
+    <t>ANNEX 1-1</t>
+  </si>
+  <si>
+    <t>slice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -404,6 +425,14 @@
       <family val="2"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -411,7 +440,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +507,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -488,10 +523,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -499,7 +535,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -511,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -522,8 +558,11 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -836,15 +875,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4690C8-E376-F64C-83C0-2939844C6F10}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -854,8 +896,20 @@
       <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>161</v>
       </c>
@@ -866,7 +920,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>162</v>
       </c>
@@ -877,7 +931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
         <v>163</v>
       </c>
@@ -888,7 +942,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>165</v>
       </c>
@@ -899,7 +953,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
         <v>166</v>
       </c>
@@ -910,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>170</v>
       </c>
@@ -921,7 +975,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="17">
         <v>174</v>
       </c>
@@ -932,7 +986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>175</v>
       </c>
@@ -943,23 +997,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="20">
+        <v>177</v>
+      </c>
+      <c r="B10" s="20">
+        <v>7</v>
+      </c>
+      <c r="C10" s="20">
+        <v>8</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="20">
+        <v>6</v>
+      </c>
+      <c r="F10" s="20">
+        <v>14</v>
+      </c>
+      <c r="G10" s="20">
+        <v>23600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="7"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{9E464BCF-13CF-634C-A550-CE15BD679836}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{119486A2-4A2B-D247-A44C-CAB1B05D3F70}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="98.6640625" customWidth="1"/>
-    <col min="3" max="3" width="249" customWidth="1"/>
+    <col min="3" max="3" width="255.6640625" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="86.5" customWidth="1"/>
     <col min="6" max="6" width="53.1640625" customWidth="1"/>
@@ -2255,6 +2343,126 @@
       <c r="G63" s="18"/>
       <c r="H63" s="18"/>
     </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="20">
+        <v>177</v>
+      </c>
+      <c r="B64" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E64" s="20">
+        <v>1</v>
+      </c>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="20">
+        <v>177</v>
+      </c>
+      <c r="B65" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E65" s="20">
+        <v>1</v>
+      </c>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="20">
+        <v>177</v>
+      </c>
+      <c r="B66" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="20">
+        <v>0</v>
+      </c>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="20">
+        <v>177</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E67" s="20">
+        <v>0</v>
+      </c>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="20">
+        <v>177</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C68" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E68" s="20">
+        <v>1</v>
+      </c>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="20">
+        <v>177</v>
+      </c>
+      <c r="B69" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C69" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E69" s="20">
+        <v>1</v>
+      </c>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2263,10 +2471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C877F0A9-3B5A-A944-83AA-53E65EA9EAD4}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView zoomScale="143" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2930,8 +3138,125 @@
       <c r="G32" s="16"/>
       <c r="H32" s="16"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="20">
+        <v>177</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="20">
+        <v>1</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="20">
+        <v>177</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="20">
+        <v>1</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="20">
+        <v>177</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E35" s="20">
+        <v>0</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="20">
+        <v>177</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="20">
+        <v>1</v>
+      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="20">
+        <v>177</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="20">
+        <v>1</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="20">
+        <v>177</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="20">
+        <v>1</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change dir name to references from paper
</commit_message>
<xml_diff>
--- a/dataset/label/legality.xlsx
+++ b/dataset/label/legality.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zachary/projects/DeepWTO/dataset/label/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B8071D-B229-9542-99AC-E74494D2C8C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0C6584-0B7C-CB44-BEBD-0B58E56FF8F8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{A0875B64-83E1-E643-88C4-98CC9A5081C5}"/>
   </bookViews>
@@ -878,7 +878,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1021,8 +1021,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>184</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>